<commit_message>
Adjust MAMBI Salinity standards to deal with single TF stations
Calculating MAMBI scores in a dataset with a single Tidal Freshwater site would cause the PCA part of the script to fail, as it needs multiple values.  The real score is calculated during the TF part of the script, but the data have to pass through the Saline part of the script first.  As such, two placeholder Tidal Freshwater values (good and bad reference) were added to the Saline Standards file.  This allows the PCA to be calculated for the lone tidal freshwater site, discard it, and then allow the rest of script to continue running.
</commit_message>
<xml_diff>
--- a/data/Pelletier2018_Standards.xlsx
+++ b/data/Pelletier2018_Standards.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\MAMBI Rollout_djg\SF Bay RMP\R Stuff\djg_MAMBI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidg\Documents\Projects\MAMBI Tool\Final MAMBI Tool\MAMBI Calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3C17130E-72DD-4ECA-9DC4-A89B8E6D0169}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A76D5BB-77C6-48C8-8BBB-B93D418A9923}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11760" activeTab="1" xr2:uid="{19F7822D-861E-47C5-865E-3854A38EE367}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{19F7822D-861E-47C5-865E-3854A38EE367}"/>
   </bookViews>
   <sheets>
     <sheet name="Saline Sites" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
   <si>
     <t>Replicate</t>
   </si>
@@ -119,6 +119,12 @@
   </si>
   <si>
     <t>SalZone</t>
+  </si>
+  <si>
+    <t>TF_bad_placeholder</t>
+  </si>
+  <si>
+    <t>TF_good_placeholder</t>
   </si>
 </sst>
 </file>
@@ -470,13 +476,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F79BC212-C50E-409F-B7B1-7774D65E439D}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -776,6 +785,46 @@
       </c>
       <c r="F15" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0.15</v>
+      </c>
+      <c r="D17">
+        <v>1.93</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -787,7 +836,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D19413A-F866-444D-A76F-41F5A3EBF3D8}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>

</xml_diff>